<commit_message>
The rotation is determined by arctangent of the dxc and dyc variables... seems to be more immune to noisy data and giving better results than the floating point variable types as in the TestCase excel file updated
</commit_message>
<xml_diff>
--- a/TestCases_04052020.xlsx
+++ b/TestCases_04052020.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="16bit fixed point " sheetId="1" r:id="rId1"/>
     <sheet name="32bit fixed point" sheetId="2" r:id="rId2"/>
     <sheet name="floating point" sheetId="3" r:id="rId3"/>
+    <sheet name="32bit Fixed Point (arctan)" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="32">
   <si>
     <t>Case Number</t>
   </si>
@@ -135,7 +136,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -151,6 +152,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -255,7 +262,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -273,6 +280,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -293,8 +304,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1499,18 +1509,18 @@
       <c r="H14" s="8"/>
     </row>
     <row r="15" spans="1:11">
-      <c r="E15" s="9" t="s">
+      <c r="E15" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="11"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="13"/>
     </row>
     <row r="16" spans="1:11" ht="32.25" customHeight="1" thickBot="1">
-      <c r="E16" s="12"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1525,8 +1535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection sqref="A1:K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1794,10 +1804,10 @@
       <c r="F8" s="2">
         <v>4</v>
       </c>
-      <c r="G8" s="15">
+      <c r="G8" s="9">
         <v>1</v>
       </c>
-      <c r="H8" s="16">
+      <c r="H8" s="10">
         <v>0</v>
       </c>
       <c r="I8" s="2" t="s">
@@ -1827,10 +1837,10 @@
       <c r="F9" s="2">
         <v>4</v>
       </c>
-      <c r="G9" s="15">
+      <c r="G9" s="9">
         <v>1</v>
       </c>
-      <c r="H9" s="16">
+      <c r="H9" s="10">
         <v>0</v>
       </c>
       <c r="I9" s="2" t="s">
@@ -1893,10 +1903,10 @@
       <c r="F11" s="2">
         <v>60</v>
       </c>
-      <c r="G11" s="15">
+      <c r="G11" s="9">
         <v>50</v>
       </c>
-      <c r="H11" s="16">
+      <c r="H11" s="10">
         <v>54</v>
       </c>
       <c r="I11" s="2" t="s">
@@ -1926,10 +1936,10 @@
       <c r="F12" s="2">
         <v>4</v>
       </c>
-      <c r="G12" s="15">
+      <c r="G12" s="9">
         <v>-12</v>
       </c>
-      <c r="H12" s="16">
+      <c r="H12" s="10">
         <v>-5</v>
       </c>
       <c r="I12" s="2" t="s">
@@ -1959,11 +1969,464 @@
       <c r="F13" s="2">
         <v>0</v>
       </c>
-      <c r="G13" s="15">
+      <c r="G13" s="9">
         <v>-7</v>
       </c>
-      <c r="H13" s="16">
+      <c r="H13" s="10">
         <v>-3</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J13" s="2">
+        <v>-3.5</v>
+      </c>
+      <c r="K13" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:K13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="51" customHeight="1">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="42" customHeight="1">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>60</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="2">
+        <v>59.9</v>
+      </c>
+      <c r="G2" s="2">
+        <v>60</v>
+      </c>
+      <c r="H2" s="17">
+        <v>60</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="2">
+        <v>60</v>
+      </c>
+      <c r="K2" s="2"/>
+    </row>
+    <row r="3" spans="1:11" ht="36.75" customHeight="1">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="2">
+        <v>4</v>
+      </c>
+      <c r="G3" s="2">
+        <v>4</v>
+      </c>
+      <c r="H3" s="17">
+        <v>4</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" s="2">
+        <v>4</v>
+      </c>
+      <c r="K3" s="2"/>
+    </row>
+    <row r="4" spans="1:11" ht="38.25" customHeight="1">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>60</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="2">
+        <v>60</v>
+      </c>
+      <c r="G4" s="2">
+        <v>60</v>
+      </c>
+      <c r="H4" s="17">
+        <v>60</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="2">
+        <v>59</v>
+      </c>
+      <c r="K4" s="2"/>
+    </row>
+    <row r="5" spans="1:11" ht="41.25" customHeight="1">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="2">
+        <v>4</v>
+      </c>
+      <c r="G5" s="2">
+        <v>2</v>
+      </c>
+      <c r="H5" s="17">
+        <v>4</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" s="2">
+        <v>3</v>
+      </c>
+      <c r="K5" s="2"/>
+    </row>
+    <row r="6" spans="1:11" ht="30" customHeight="1">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
+        <v>2</v>
+      </c>
+      <c r="H6" s="17">
+        <v>1</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="K6" s="2"/>
+    </row>
+    <row r="7" spans="1:11" ht="33" customHeight="1">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>60</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="2">
+        <v>60</v>
+      </c>
+      <c r="G7" s="2">
+        <v>60</v>
+      </c>
+      <c r="H7" s="17">
+        <v>60</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J7" s="2">
+        <v>60</v>
+      </c>
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="1:11" ht="30.75" customHeight="1">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2">
+        <v>4</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="2">
+        <v>4</v>
+      </c>
+      <c r="G8" s="2">
+        <v>4</v>
+      </c>
+      <c r="H8" s="17">
+        <v>3</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J8" s="2">
+        <v>2</v>
+      </c>
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" spans="1:11" ht="33" customHeight="1">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2">
+        <v>4</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="2">
+        <v>4</v>
+      </c>
+      <c r="G9" s="2">
+        <v>4</v>
+      </c>
+      <c r="H9" s="17">
+        <v>3</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J9" s="2">
+        <v>2</v>
+      </c>
+      <c r="K9" s="2"/>
+    </row>
+    <row r="10" spans="1:11" ht="27" customHeight="1">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0</v>
+      </c>
+      <c r="G10" s="2">
+        <v>4</v>
+      </c>
+      <c r="H10" s="17">
+        <v>1</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J10" s="2">
+        <v>1</v>
+      </c>
+      <c r="K10" s="2"/>
+    </row>
+    <row r="11" spans="1:11" ht="30.75" customHeight="1">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2">
+        <v>60</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="2">
+        <v>60</v>
+      </c>
+      <c r="G11" s="2">
+        <v>56</v>
+      </c>
+      <c r="H11" s="17">
+        <v>56</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J11" s="2">
+        <v>59</v>
+      </c>
+      <c r="K11" s="2"/>
+    </row>
+    <row r="12" spans="1:11" ht="26.25" customHeight="1">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2">
+        <v>4</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="2">
+        <v>4</v>
+      </c>
+      <c r="G12" s="2">
+        <v>6</v>
+      </c>
+      <c r="H12" s="17">
+        <v>1</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J12" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="1:11" ht="25.5" customHeight="1">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0</v>
+      </c>
+      <c r="G13" s="2">
+        <v>6</v>
+      </c>
+      <c r="H13" s="17">
+        <v>2</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
The thershold for testing rotations is changed from pi/2 to 2 in radians which did have some improvements in the 14400 test cases...
</commit_message>
<xml_diff>
--- a/TestCases_04052020.xlsx
+++ b/TestCases_04052020.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="39">
   <si>
     <t>Case Number</t>
   </si>
@@ -113,6 +113,27 @@
   </si>
   <si>
     <t>ExpectedOctave Result</t>
+  </si>
+  <si>
+    <t>56/62</t>
+  </si>
+  <si>
+    <t>Every Sample</t>
+  </si>
+  <si>
+    <t>56/58</t>
+  </si>
+  <si>
+    <t>6/-2</t>
+  </si>
+  <si>
+    <t>6/-6</t>
+  </si>
+  <si>
+    <t>1/1--</t>
+  </si>
+  <si>
+    <t>2/-4</t>
   </si>
 </sst>
 </file>
@@ -262,7 +283,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -286,6 +307,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -304,7 +328,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1509,18 +1533,18 @@
       <c r="H14" s="8"/>
     </row>
     <row r="15" spans="1:11">
-      <c r="E15" s="11" t="s">
+      <c r="E15" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="14"/>
     </row>
     <row r="16" spans="1:11" ht="32.25" customHeight="1" thickBot="1">
-      <c r="E16" s="14"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="16"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1992,8 +2016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H13"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="J12" sqref="A12:J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2062,11 +2086,11 @@
       <c r="G2" s="2">
         <v>60</v>
       </c>
-      <c r="H2" s="17">
+      <c r="H2" s="11">
         <v>60</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="J2" s="2">
         <v>60</v>
@@ -2095,11 +2119,11 @@
       <c r="G3" s="2">
         <v>4</v>
       </c>
-      <c r="H3" s="17">
+      <c r="H3" s="11">
         <v>4</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="J3" s="2">
         <v>4</v>
@@ -2128,11 +2152,11 @@
       <c r="G4" s="2">
         <v>60</v>
       </c>
-      <c r="H4" s="17">
+      <c r="H4" s="11">
         <v>60</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="J4" s="2">
         <v>59</v>
@@ -2161,11 +2185,11 @@
       <c r="G5" s="2">
         <v>2</v>
       </c>
-      <c r="H5" s="17">
+      <c r="H5" s="11">
         <v>4</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="J5" s="2">
         <v>3</v>
@@ -2194,11 +2218,11 @@
       <c r="G6" s="2">
         <v>2</v>
       </c>
-      <c r="H6" s="17">
+      <c r="H6" s="11">
         <v>1</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="J6" s="2">
         <v>0.5</v>
@@ -2227,11 +2251,11 @@
       <c r="G7" s="2">
         <v>60</v>
       </c>
-      <c r="H7" s="17">
+      <c r="H7" s="11">
         <v>60</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="J7" s="2">
         <v>60</v>
@@ -2260,11 +2284,11 @@
       <c r="G8" s="2">
         <v>4</v>
       </c>
-      <c r="H8" s="17">
+      <c r="H8" s="11">
         <v>3</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="J8" s="2">
         <v>2</v>
@@ -2293,11 +2317,11 @@
       <c r="G9" s="2">
         <v>4</v>
       </c>
-      <c r="H9" s="17">
+      <c r="H9" s="11">
         <v>3</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="J9" s="2">
         <v>2</v>
@@ -2326,11 +2350,11 @@
       <c r="G10" s="2">
         <v>4</v>
       </c>
-      <c r="H10" s="17">
+      <c r="H10" s="11">
         <v>1</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="J10" s="2">
         <v>1</v>
@@ -2356,14 +2380,14 @@
       <c r="F11" s="2">
         <v>60</v>
       </c>
-      <c r="G11" s="2">
-        <v>56</v>
-      </c>
-      <c r="H11" s="17">
-        <v>56</v>
+      <c r="G11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>32</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="J11" s="2">
         <v>59</v>
@@ -2389,14 +2413,14 @@
       <c r="F12" s="2">
         <v>4</v>
       </c>
-      <c r="G12" s="2">
-        <v>6</v>
-      </c>
-      <c r="H12" s="17">
-        <v>1</v>
+      <c r="G12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H12" s="18" t="s">
+        <v>37</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="J12" s="2">
         <v>1.5</v>
@@ -2422,14 +2446,14 @@
       <c r="F13" s="2">
         <v>0</v>
       </c>
-      <c r="G13" s="2">
-        <v>6</v>
-      </c>
-      <c r="H13" s="17">
-        <v>2</v>
+      <c r="G13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>38</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="J13" s="2">
         <v>-3.5</v>

</xml_diff>